<commit_message>
Last final Ultimate commit
</commit_message>
<xml_diff>
--- a/exam_planner_backend/app/static/templates/excel/utilizatori_SG.xlsx
+++ b/exam_planner_backend/app/static/templates/excel/utilizatori_SG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cirla\Desktop\exam_panner\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cirla\Desktop\an I\sem 2\TWAAOS\exam_planner\exam_planner_backend\app\static\templates\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CAC692-B2DB-40BE-B088-0739CA30E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C93553-EF3E-4A02-A259-BC4E8DDBFA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="969" windowWidth="24686" windowHeight="13165" xr2:uid="{C7D265A7-CAB7-46D4-8388-D9FD25EFBA84}"/>
+    <workbookView xWindow="754" yWindow="754" windowWidth="24686" windowHeight="13106" xr2:uid="{C7D265A7-CAB7-46D4-8388-D9FD25EFBA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -42,34 +42,19 @@
     <t>year_of_study</t>
   </si>
   <si>
-    <t>rebeca polocoser</t>
-  </si>
-  <si>
-    <t>rebeca@gmail.com</t>
-  </si>
-  <si>
     <t>SIC</t>
   </si>
   <si>
-    <t>alexandra</t>
-  </si>
-  <si>
-    <t>alexandra@gmail.com</t>
-  </si>
-  <si>
     <t>ancuta cirlan</t>
   </si>
   <si>
     <t>ancuta.cirlan1@student.usv.ro</t>
   </si>
   <si>
-    <t>maria bersa</t>
-  </si>
-  <si>
-    <t>maria@gmail.com</t>
-  </si>
-  <si>
-    <t>sic</t>
+    <t>maria maria</t>
+  </si>
+  <si>
+    <t>maria@student.usv.ro</t>
   </si>
 </sst>
 </file>
@@ -432,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581A4D83-A5D0-45A5-9B7F-D985BF2B0AE1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -466,16 +451,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>3711</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>3112</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -489,46 +474,19 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>3113</v>
+        <v>3114</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>3114</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F67FC070-DF14-4638-9F86-3D46C16D1B11}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{21893504-89E5-4CA1-87F4-0B6A67928783}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{AF04DE86-BB6B-4B62-9BA4-391A70916D8E}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{25C4E25A-32E2-42C2-B5D3-A6D7C6B2D122}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AF04DE86-BB6B-4B62-9BA4-391A70916D8E}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{25C4E25A-32E2-42C2-B5D3-A6D7C6B2D122}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>